<commit_message>
Added Hand written images for explanation
</commit_message>
<xml_diff>
--- a/ANOVA_questions/Practice_Datasets.xlsx
+++ b/ANOVA_questions/Practice_Datasets.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\STUDY\Projects\Maths_for_ML\Statistics_for_ML\ANOVA_questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\Git\Statistical_testing_python\ANOVA_questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E8F8CE-0415-4996-B091-377F61A704D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772FFE82-7D73-4C5D-84CE-2F6A9DF3A52C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{30E246B5-9478-4BB9-8B75-021E5B744B1D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" activeTab="1" xr2:uid="{30E246B5-9478-4BB9-8B75-021E5B744B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVA_8.2.1" sheetId="1" r:id="rId1"/>
+    <sheet name="ANOVA_8.2.2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>LUPUS</t>
+  </si>
+  <si>
+    <t>PMRTA</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,17 +111,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,1177 +439,1177 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14626B22-5DB1-49BC-BF1B-F2DC02D255FC}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="3">
         <v>30</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2">
+      <c r="B1" s="3"/>
+      <c r="C1" s="1">
         <v>60</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="3">
         <v>90</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="1">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>-1E-3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>-7.0000000000000001E-3</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>0.55800000000000005</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>0.05</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1.0609999999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.01</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.52900000000000003</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>0.27200000000000002</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1.04</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.26900000000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>-3.9E-2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0.52400000000000002</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0.28699999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>0.55200000000000005</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1.097</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>5.5E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>-0.08</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>0.55500000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>1.1160000000000001</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1.08</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1.103</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.105</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.108</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>-0.11799999999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>0.53900000000000003</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>1.1180000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>2.7330000000000001</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>1.0509999999999999</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>2.7269999999999999</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.27200000000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.27800000000000002</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>-0.29099999999999998</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.53600000000000003</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>2.7629999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>0</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>-2E-3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.55300000000000005</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>-0.60199999999999998</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>0.55700000000000005</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1.075</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.84</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>-0.88400000000000001</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>0.54400000000000004</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>0.27500000000000002</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>1.0349999999999999</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.27100000000000002</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1.1060000000000001</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>-1.1759999999999999</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>0.53900000000000003</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>0.27700000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>0.55600000000000005</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>1.0960000000000001</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1.647</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1.65</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>-1.7250000000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>1.109</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>1.097</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>2.7280000000000002</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>2.7290000000000001</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>1.085</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>1.113</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>2.7229999999999999</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1.0960000000000001</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>2.7250000000000001</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>-1E-3</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>1.07</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>2.7589999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1.1080000000000001</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>-2.3E-2</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>5.5E-2</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>1.099</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>2.7E-2</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>-3.6999999999999998E-2</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>-0.06</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>1.069</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>0.27300000000000002</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>1.089</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>0.27</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>-4.5999999999999999E-2</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>-9.7000000000000003E-2</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>1.0449999999999999</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>0.28599999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>0.55300000000000005</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>1.107</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>0.55300000000000005</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>0.111</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>-0.13400000000000001</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>-0.32</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>0.56399999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>1.0940000000000001</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>0.27600000000000002</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>-0.29699999999999999</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>-0.59299999999999997</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>1.0660000000000001</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>1.1040000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>2.7130000000000001</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>1.0920000000000001</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>2.7269999999999999</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>-0.58899999999999997</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>-0.84</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>1.0369999999999999</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>2.76</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>1.0920000000000001</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0.83199999999999996</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>-0.876</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>-1.1679999999999999</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>2.7280000000000002</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>-6.6000000000000003E-2</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>-7.4999999999999997E-2</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>1.099</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>-1.157</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>-1.76</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>2.694</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>-0.06</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>-0.25800000000000001</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1.121</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>1.651</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>-1.7549999999999999</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>2.6629999999999998</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>-0.28899999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>-0.58099999999999996</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>1.1060000000000001</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>-0.58499999999999996</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>2.7360000000000002</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>-2.8620000000000001</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>0.56599999999999995</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>2.7240000000000002</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>-0.58499999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>-1.1619999999999999</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>1.135</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>-1.1679999999999999</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>0.56399999999999995</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>0</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>1.1160000000000001</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>2.6930000000000001</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>-1.18</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>1.143</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>0.55600000000000005</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>0.245</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>2.762</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>2.67</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>-4.4999999999999998E-2</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>1.1060000000000001</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>0.497</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>0.56299999999999994</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>2.72</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>-3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>-0.27400000000000002</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>1.135</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>-0.25800000000000001</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>0.56699999999999995</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>2.6880000000000002</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>-0.29499999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>-0.60399999999999998</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>1.1559999999999999</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>-0.54800000000000004</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>0.55900000000000005</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>0.248</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>2.66</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>-0.57899999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>-1.143</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>1.1120000000000001</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>-1.1870000000000001</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>0.498</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>0.56100000000000005</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>0.55600000000000005</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>-1.165</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>1.9E-2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>1.107</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>-1.9E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>-0.05</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>1.107</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>0.246</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>0.55800000000000005</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>0.55700000000000005</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>-5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>1.107</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>-0.29199999999999998</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>1.1020000000000001</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>-0.27</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>-0.60699999999999998</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>-0.54200000000000004</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>1.1120000000000001</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>0.56599999999999995</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>0.56399999999999995</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>-0.57899999999999996</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>-1.1639999999999999</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>1.117</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>-1.1890000000000001</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>1.103</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>0.26200000000000001</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>0.55500000000000005</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>-1.1619999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>1.105</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>1.101</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>0.52700000000000002</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>1.107</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>0.55100000000000005</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2">
         <v>1.103</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2">
         <v>1.1140000000000001</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>1.1040000000000001</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>0.56299999999999994</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2">
         <v>1.095</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>0.26</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>1.109</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>0.55900000000000005</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>0.52300000000000002</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>1.1080000000000001</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>1.113</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2">
         <v>2.7389999999999999</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>1.1060000000000001</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>1.1140000000000001</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2">
         <v>2.7210000000000001</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>0.26100000000000001</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>1.1020000000000001</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>1.101</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2">
         <v>2.6869999999999998</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>0.52300000000000002</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>1.111</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>1.113</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2">
         <v>2.7320000000000002</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>2.6960000000000002</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>1.1020000000000001</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>1.113</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2">
         <v>2.702</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>2.6640000000000001</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>1.107</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>1.097</v>
       </c>
-      <c r="H43" s="3"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2">
         <v>2.66</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>2.722</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>2.7349999999999999</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>1.1160000000000001</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2">
         <v>2.7429999999999999</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>2.6859999999999999</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>2.7330000000000001</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="2">
         <v>1.1120000000000001</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2">
         <v>2.6869999999999998</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>2.661</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <v>2.6589999999999998</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="2">
         <v>1.0980000000000001</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2">
         <v>2.6560000000000001</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>0.54800000000000004</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <v>2.7269999999999999</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <v>2.7320000000000002</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2">
         <v>2.7330000000000001</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>2.7389999999999999</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <v>0.54200000000000004</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <v>2.722</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2">
         <v>2.7309999999999999</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>2.742</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <v>0.55600000000000005</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <v>2.734</v>
       </c>
-      <c r="H49" s="3"/>
+      <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2">
         <v>2.7280000000000002</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="2">
         <v>2.7469999999999999</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1601,4 +1619,425 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518163DB-AF9B-48D5-9D71-3AC495ACBE19}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>11.090999999999999</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7.4119999999999999</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.9609999999999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-3.669</v>
+      </c>
+      <c r="E2" s="4">
+        <v>11.146000000000001</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2.9369999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>24.414000000000001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5.5590000000000002</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-7.8159999999999998</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.83799999999999997</v>
+      </c>
+      <c r="F3" s="4">
+        <v>15.968</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>10.025</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8.3940000000000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.5629999999999997</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4.0819999999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5.3490000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>-3.1560000000000001</v>
+      </c>
+      <c r="B5" s="4">
+        <v>-3.5270000000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2.8319999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.6449999999999996</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.7190000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>6.835</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4.8390000000000004</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-1.369</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-0.185</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4.3289999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.4450000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>3.3210000000000002</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="C7" s="4">
+        <v>11.288</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.302</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.234</v>
+      </c>
+      <c r="F7" s="4">
+        <v>20.242999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-3.9329999999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.9969999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.2990000000000004</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-2.8170000000000002</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>-1.8640000000000001</v>
+      </c>
+      <c r="B9" s="4">
+        <v>9.6690000000000005</v>
+      </c>
+      <c r="C9" s="4">
+        <v>7.26</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10.734</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3.544</v>
+      </c>
+      <c r="F9" s="4">
+        <v>8.9920000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>5.3860000000000001</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4.6589999999999998</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5.5460000000000003</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.399</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4.16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>3.8679999999999999</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.137</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
+        <v>0.497</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F11" s="4">
+        <v>25.655000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>6.2089999999999996</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7.5209999999999999</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-0.247</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>-5.64</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5.3719999999999999</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>3.5139999999999998</v>
+      </c>
+      <c r="B14" s="4">
+        <v>-8.6839999999999993</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.7210000000000001</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>-2.3079999999999998</v>
+      </c>
+      <c r="B15" s="4">
+        <v>-0.372</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4">
+        <v>9.3539999999999992</v>
+      </c>
+      <c r="E15" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15.981</v>
+      </c>
+      <c r="B16" s="4">
+        <v>21.311</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
+        <v>2.61</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10.82</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>-9.6460000000000008</v>
+      </c>
+      <c r="B17" s="4">
+        <v>10.831</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4">
+        <v>5.6820000000000004</v>
+      </c>
+      <c r="E17" s="4">
+        <v>7.28</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>5.1879999999999997</v>
+      </c>
+      <c r="B18" s="4">
+        <v>3.351</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
+        <v>6.6050000000000004</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>-1.8919999999999999</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9.5570000000000004</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4">
+        <v>7.5069999999999997</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>16.553000000000001</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4">
+        <v>5.0750000000000002</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>12.766999999999999</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4">
+        <v>3.4809999999999999</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <v>15.853</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>